<commit_message>
add new fields and corrections
</commit_message>
<xml_diff>
--- a/static/excel/pool-importvorlage-komplett.xlsx
+++ b/static/excel/pool-importvorlage-komplett.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sgr/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEEE01D-64BF-42DB-97FB-1F35D61B039F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E074CB-8027-0C4A-BC96-537EBBBD922D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1430" yWindow="1400" windowWidth="34140" windowHeight="19430" xr2:uid="{D7DA82DE-661B-4434-8FCB-AD97B6E46B4F}"/>
+    <workbookView xWindow="51620" yWindow="620" windowWidth="34140" windowHeight="19440" xr2:uid="{D7DA82DE-661B-4434-8FCB-AD97B6E46B4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
   <si>
     <t>number</t>
   </si>
@@ -255,6 +255,30 @@
   </si>
   <si>
     <t>beliebigerVariantencode</t>
+  </si>
+  <si>
+    <t>isEcoProduct</t>
+  </si>
+  <si>
+    <t>0 oder leer = Nein, 1 = Ja</t>
+  </si>
+  <si>
+    <t>unit1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verpackungseinheit1 </t>
+  </si>
+  <si>
+    <t>minimumQuantity1</t>
+  </si>
+  <si>
+    <t>maximumQuantity1</t>
+  </si>
+  <si>
+    <t>mind. Anzahl Bestelleinheiten</t>
+  </si>
+  <si>
+    <t>max. Anzahl Bestelleinheiten</t>
   </si>
 </sst>
 </file>
@@ -311,7 +335,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -327,7 +351,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -623,22 +647,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68064CE6-FD76-4DBC-9329-3242BDA4121F}">
-  <dimension ref="A1:AX2"/>
+  <dimension ref="A1:BB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="AY2" sqref="AY2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="22.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="38.90625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="36.90625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="36.83203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -724,73 +749,85 @@
         <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -867,54 +904,66 @@
         <v>59</v>
       </c>
       <c r="AC2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD2" t="s">
         <v>60</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>61</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <v>46010305</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>62</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>63</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>64</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>65</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>66</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>68</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>67</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>69</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>70</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AU2" t="s">
         <v>71</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AV2" t="s">
         <v>70</v>
       </c>
-      <c r="AV2">
+      <c r="AW2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ2">
         <v>8.5</v>
       </c>
-      <c r="AW2" s="3">
+      <c r="BA2" s="3">
         <v>45170</v>
       </c>
-      <c r="AX2" s="3">
+      <c r="BB2" s="3">
         <v>45291</v>
       </c>
     </row>
@@ -925,6 +974,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BA0AE64D09535C45B43E32951E7FE192" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="dc5367d52721b3cc686ff2a4502c4b22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="972a4302-61b6-4e60-8451-b9c9ef50fbef" xmlns:ns3="c9de2a3f-a2ad-4682-ba79-07e79da285ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6be2ebb54767e97eb371acbf5d625405" ns2:_="" ns3:_="">
     <xsd:import namespace="972a4302-61b6-4e60-8451-b9c9ef50fbef"/>
@@ -1167,19 +1225,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE263A7-639F-4BE6-96CD-2C6799C9EA64}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEF06674-B273-439D-B6E9-31FC69439600}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEF06674-B273-439D-B6E9-31FC69439600}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE263A7-639F-4BE6-96CD-2C6799C9EA64}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="972a4302-61b6-4e60-8451-b9c9ef50fbef"/>
+    <ds:schemaRef ds:uri="c9de2a3f-a2ad-4682-ba79-07e79da285ff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>